<commit_message>
fix typo in detector test results
</commit_message>
<xml_diff>
--- a/Test/grader_detector_test_v4_all_typefixed.xlsx
+++ b/Test/grader_detector_test_v4_all_typefixed.xlsx
@@ -3274,8 +3274,8 @@
   <dimension ref="A1:P935"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A830" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E849" sqref="E849"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L178" sqref="L178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8883,8 +8883,7 @@
       </c>
       <c r="G178" s="5"/>
       <c r="H178" s="9"/>
-      <c r="K178" s="5"/>
-      <c r="M178">
+      <c r="K178" s="5">
         <v>1</v>
       </c>
       <c r="N178" s="8"/>
@@ -9257,10 +9256,10 @@
         <v>20</v>
       </c>
       <c r="C190" s="3"/>
-      <c r="D190" s="4"/>
-      <c r="E190" s="5">
-        <v>1</v>
-      </c>
+      <c r="D190" s="4">
+        <v>1</v>
+      </c>
+      <c r="E190" s="5"/>
       <c r="G190" s="5"/>
       <c r="K190" s="5"/>
       <c r="M190">
@@ -9348,10 +9347,10 @@
         <v>20</v>
       </c>
       <c r="C193" s="3"/>
-      <c r="D193" s="4"/>
-      <c r="E193" s="5">
-        <v>1</v>
-      </c>
+      <c r="D193" s="4">
+        <v>1</v>
+      </c>
+      <c r="E193" s="5"/>
       <c r="G193" s="5"/>
       <c r="K193" s="5"/>
       <c r="M193">

</xml_diff>

<commit_message>
fix typo in detector test results v2
</commit_message>
<xml_diff>
--- a/Test/grader_detector_test_v4_all_typefixed.xlsx
+++ b/Test/grader_detector_test_v4_all_typefixed.xlsx
@@ -3275,7 +3275,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L178" sqref="L178"/>
+      <selection pane="bottomLeft" activeCell="K178" sqref="K178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8876,11 +8876,11 @@
       <c r="B178">
         <v>19</v>
       </c>
-      <c r="C178" s="3"/>
+      <c r="C178" s="3">
+        <v>1</v>
+      </c>
       <c r="D178" s="4"/>
-      <c r="E178" s="5">
-        <v>1</v>
-      </c>
+      <c r="E178" s="5"/>
       <c r="G178" s="5"/>
       <c r="H178" s="9"/>
       <c r="K178" s="5">

</xml_diff>